<commit_message>
Implement DFS solver and enhance core gameplay features
Core Gameplay & UI/UX Enhancements:
- New Game Functionality
- Re-runnable Solve Button
- Input Validation
- Auto-Clear Invalid Guesses
- Settings Persistence Fix
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -1036,7 +1036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -1339,6 +1339,396 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0977</v>
+      </c>
+      <c r="C12" t="n">
+        <v>84</v>
+      </c>
+      <c r="D12" t="n">
+        <v>57</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LOPEZ</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>AARON, LEGAL, PEERS, BLEND, CHEAP, CLERK, DELAY, EQUAL, IDEAL, MEDAL, METAL, SPEAK, SPEND, SPENT, SPERM, SPINE, STEAL, EVENT, EVERY, SCENE, TEENS, THERE, WHERE, LUCAS, LYING, BEING, BLIND, BLINK, CHEAT, ESSAY, FIBRE, IDEAS, ISLAM, MYERS, QUERY, SHINE, STEAM, TEXAS, USERS, USUAL, VEGAS, VITAL, WEIRD, WHEAT, DUBAI, DYING, SHIRT, SIGNS, SKINS, SKIRT, SQUAD, SWING, THING, THINK, THIRD, TWINS, USING</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="C13" t="n">
+        <v>84</v>
+      </c>
+      <c r="D13" t="n">
+        <v>57</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LOPEZ</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>AARON, LEGAL, PEERS, BLEND, CHEAP, CLERK, DELAY, EQUAL, IDEAL, MEDAL, METAL, SPEAK, SPEND, SPENT, SPERM, SPINE, STEAL, EVENT, EVERY, SCENE, TEENS, THERE, WHERE, LUCAS, LYING, BEING, BLIND, BLINK, CHEAT, ESSAY, FIBRE, IDEAS, ISLAM, MYERS, QUERY, SHINE, STEAM, TEXAS, USERS, USUAL, VEGAS, VITAL, WEIRD, WHEAT, DUBAI, DYING, SHIRT, SIGNS, SKINS, SKIRT, SQUAD, SWING, THING, THINK, THIRD, TWINS, USING</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.09719999999999999</v>
+      </c>
+      <c r="C14" t="n">
+        <v>84</v>
+      </c>
+      <c r="D14" t="n">
+        <v>57</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LOPEZ</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>AARON, LEGAL, PEERS, BLEND, CHEAP, CLERK, DELAY, EQUAL, IDEAL, MEDAL, METAL, SPEAK, SPEND, SPENT, SPERM, SPINE, STEAL, EVENT, EVERY, SCENE, TEENS, THERE, WHERE, LUCAS, LYING, BEING, BLIND, BLINK, CHEAT, ESSAY, FIBRE, IDEAS, ISLAM, MYERS, QUERY, SHINE, STEAM, TEXAS, USERS, USUAL, VEGAS, VITAL, WEIRD, WHEAT, DUBAI, DYING, SHIRT, SIGNS, SKINS, SKIRT, SQUAD, SWING, THING, THINK, THIRD, TWINS, USING</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C15" t="n">
+        <v>233</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LIKED</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>AARON, LIKED</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.1069</v>
+      </c>
+      <c r="C16" t="n">
+        <v>101</v>
+      </c>
+      <c r="D16" t="n">
+        <v>57</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>POSTS</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>AARON, SPENT, PEERS, ESSAY, SIGNS, SKINS, TEENS, TEXAS, TWINS, USERS, SHIRT, SKIRT, SPEAK, SPEND, SPERM, SPINE, STEAL, STEAM, IDEAS, LUCAS, MYERS, VEGAS, CHEAP, CHEAT, EVENT, ISLAM, METAL, SCENE, SHINE, SQUAD, SWING, THERE, THING, THINK, THIRD, USING, USUAL, VITAL, WHEAT, BEING, BLEND, BLIND, BLINK, CLERK, DELAY, DUBAI, DYING, EQUAL, EVERY, FIBRE, IDEAL, LEGAL, LYING, MEDAL, QUERY, WEIRD, WHERE</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0322</v>
+      </c>
+      <c r="C17" t="n">
+        <v>19</v>
+      </c>
+      <c r="D17" t="n">
+        <v>19</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>DAIRY</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>AARON, DANNY, CANDY, HANDY, SANDY, DANCE, FANCY, BANDS, HANDS, LANDS, PANIC, BANKS, JANET, LANCE, LANES, PANEL, PANTS, TANKS, WANTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>APART</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>AARON</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.0135</v>
+      </c>
+      <c r="C19" t="n">
+        <v>11</v>
+      </c>
+      <c r="D19" t="n">
+        <v>9</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>ALIAS</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>AARON, ARISE, ANIME, ANGEL, ANGLE, ANNIE, ANNEX, ARGUE, ARMED</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.0186</v>
+      </c>
+      <c r="C20" t="n">
+        <v>12</v>
+      </c>
+      <c r="D20" t="n">
+        <v>12</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>INTER</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>AARON, TUNER, BLAIR, CHAIR, CHOIR, BINGO, KENYA, KINDA, LINDA, FLOUR, IDAHO, PLAZA</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.09370000000000001</v>
+      </c>
+      <c r="C21" t="n">
+        <v>107</v>
+      </c>
+      <c r="D21" t="n">
+        <v>57</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>COMIC</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>AARON, ISLAM, CHEAP, CHEAT, CLERK, BEING, BLIND, BLINK, DUBAI, DYING, FIBRE, IDEAL, IDEAS, LUCAS, LYING, MEDAL, METAL, MYERS, SCENE, SHINE, SHIRT, SIGNS, SKINS, SKIRT, SPERM, SPINE, STEAM, SWING, THING, THINK, THIRD, TWINS, USING, VITAL, WEIRD, BLEND, DELAY, EQUAL, ESSAY, EVENT, EVERY, LEGAL, PEERS, QUERY, SPEAK, SPEND, SPENT, SQUAD, STEAL, TEENS, TEXAS, THERE, USERS, USUAL, VEGAS, WHEAT, WHERE</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C22" t="n">
+        <v>233</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>SILLY</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>AARON, SILLY</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="C23" t="n">
+        <v>233</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>FEELS</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>AARON, FEELS</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.0335</v>
+      </c>
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="n">
+        <v>21</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LEAVE</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>AARON, OLIVE, REBEL, NEEDS, NEWLY, REFER, REPLY, RESET, RIVER, RULED, RULES, OXIDE, REMIX, RIDGE, RIDER, RIDES, NIGHT, OUGHT, RIGHT, RISKS, RUGBY</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="C25" t="n">
+        <v>22</v>
+      </c>
+      <c r="D25" t="n">
+        <v>21</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LEAVE</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>AARON, OLIVE, REBEL, NEEDS, NEWLY, REFER, REPLY, RESET, RIVER, RULED, RULES, OXIDE, REMIX, RIDGE, RIDER, RIDES, NIGHT, OUGHT, RIGHT, RISKS, RUGBY</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.1002</v>
+      </c>
+      <c r="C26" t="n">
+        <v>71</v>
+      </c>
+      <c r="D26" t="n">
+        <v>62</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>DROPS</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>AARON, SPORT, SWORD, SCORE, SHORE, SHORT, STORE, STORM, STORY, SHARP, SPARC, SPARE, STARS, ICONS, LIONS, TIONS, BEARS, BLOND, DIARY, FEARS, GLORY, IVORY, PHONE, PLANS, STONE, TEARS, WHORE, YEARS, GUARD, HEARD, PEARL, SCARY, SHARE, SHARK, SMART, SPANK, STAND, START, BEANS, CLONE, DIANE, EBONY, EVANS, FLOAT, JEANS, LEONE, MEANS, THONG, CHARM, CHART, CLARK, GENRE, HEART, HENRY, ISAAC, PLANE, PLANT, BLANK, FINAL, GIANT, MEANT, THANK</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>